<commit_message>
Homologación de precios de insumos finalizada. Continúa actualización de datos.
</commit_message>
<xml_diff>
--- a/data/precios-combustibles.xlsx
+++ b/data/precios-combustibles.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27204"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28120"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a98dfaf1ce87dfc/DataScience/Proyectos/time-series-fertilizer-price-predictor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{DF7195F7-C5FE-439E-823C-FADB8615127D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{747FB6D6-DD58-431A-9C23-D389118B8102}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{DF7195F7-C5FE-439E-823C-FADB8615127D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98E056B3-E409-42F7-9730-089C11C0F51C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4CDCA299-7EAA-4C2C-BCA1-BD2F6388072C}"/>
   </bookViews>
   <sheets>
     <sheet name="precios_combustibles" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -62,7 +59,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -131,11 +128,11 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -162,46 +159,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="CONTENIDO"/>
-      <sheetName val="1. NACIONAL"/>
-      <sheetName val="2. REGION SIERRA"/>
-      <sheetName val="3. REGION COSTA"/>
-      <sheetName val="4. Guayaquil"/>
-      <sheetName val="5. Esmeraldas"/>
-      <sheetName val="6. Machala"/>
-      <sheetName val="7. Manta"/>
-      <sheetName val="8. Sto. Domingo"/>
-      <sheetName val="9. Quito"/>
-      <sheetName val="10. Loja"/>
-      <sheetName val="11. Cuenca"/>
-      <sheetName val="12. Ambato"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -521,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75819FD-9712-41C2-89A0-7D007E4405A1}">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="9.6" x14ac:dyDescent="0.2"/>
@@ -537,7 +494,7 @@
     <col min="6" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2371,6 +2328,159 @@
       </c>
       <c r="E108" s="6">
         <v>201.15519115802101</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
+        <v>45261</v>
+      </c>
+      <c r="B109" s="5">
+        <v>168.20156001145301</v>
+      </c>
+      <c r="C109" s="5">
+        <v>159.035415834426</v>
+      </c>
+      <c r="D109" s="5">
+        <v>157.98174249704101</v>
+      </c>
+      <c r="E109" s="5">
+        <v>182.72643848899901</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="3">
+        <v>45292</v>
+      </c>
+      <c r="B110" s="5">
+        <v>168.20156001145301</v>
+      </c>
+      <c r="C110" s="5">
+        <v>159.035415834426</v>
+      </c>
+      <c r="D110" s="5">
+        <v>157.98174249704101</v>
+      </c>
+      <c r="E110" s="5">
+        <v>171.602023972756</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>45323</v>
+      </c>
+      <c r="B111" s="5">
+        <v>168.20156001145301</v>
+      </c>
+      <c r="C111" s="5">
+        <v>159.035415834426</v>
+      </c>
+      <c r="D111" s="5">
+        <v>157.98174249704101</v>
+      </c>
+      <c r="E111" s="5">
+        <v>174.91479838073499</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
+        <v>45352</v>
+      </c>
+      <c r="B112" s="5">
+        <v>168.20156001145301</v>
+      </c>
+      <c r="C112" s="5">
+        <v>159.035415834426</v>
+      </c>
+      <c r="D112" s="5">
+        <v>157.98174249704101</v>
+      </c>
+      <c r="E112" s="5">
+        <v>181.495851693942</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="3">
+        <v>45383</v>
+      </c>
+      <c r="B113" s="5">
+        <v>173.00731886892299</v>
+      </c>
+      <c r="C113" s="5">
+        <v>163.67394879626301</v>
+      </c>
+      <c r="D113" s="5">
+        <v>162.58954331987201</v>
+      </c>
+      <c r="E113" s="5">
+        <v>190.96306729767201</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="3">
+        <v>45413</v>
+      </c>
+      <c r="B114" s="5">
+        <v>173.00731886892299</v>
+      </c>
+      <c r="C114" s="5">
+        <v>163.673948796264</v>
+      </c>
+      <c r="D114" s="5">
+        <v>162.58954331987201</v>
+      </c>
+      <c r="E114" s="5">
+        <v>196.322380513197</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="3">
+        <v>45444</v>
+      </c>
+      <c r="B115" s="5">
+        <v>173.00731886892299</v>
+      </c>
+      <c r="C115" s="5">
+        <v>165.137198067111</v>
+      </c>
+      <c r="D115" s="5">
+        <v>164.66692458275401</v>
+      </c>
+      <c r="E115" s="5">
+        <v>194.93070915982</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
+        <v>45474</v>
+      </c>
+      <c r="B116" s="5">
+        <v>173.00731886892299</v>
+      </c>
+      <c r="C116" s="5">
+        <v>181.52968459686701</v>
+      </c>
+      <c r="D116" s="5">
+        <v>180.19666404162999</v>
+      </c>
+      <c r="E116" s="5">
+        <v>189.946264977749</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="3">
+        <v>45505</v>
+      </c>
+      <c r="B117" s="5">
+        <v>173.00731886892299</v>
+      </c>
+      <c r="C117" s="5">
+        <v>183.02580491190699</v>
+      </c>
+      <c r="D117" s="5">
+        <v>181.74241763149001</v>
+      </c>
+      <c r="E117" s="5">
+        <v>188.746081090817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>